<commit_message>
updated to new byct_v3
</commit_message>
<xml_diff>
--- a/Data/市领导数据/人民网-市长-V1.xlsx
+++ b/Data/市领导数据/人民网-市长-V1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1895" uniqueCount="1030">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1910" uniqueCount="1030">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -964,13 +964,13 @@
     <t>齐齐哈尔</t>
   </si>
   <si>
-    <t xml:space="preserve">　　张之政</t>
+    <t>张之政</t>
   </si>
   <si>
     <t>郑艺</t>
   </si>
   <si>
-    <t xml:space="preserve">　　杨军</t>
+    <t>杨军</t>
   </si>
   <si>
     <t>王喜良</t>
@@ -991,13 +991,13 @@
     <t>费东斌</t>
   </si>
   <si>
-    <t xml:space="preserve">　　唐毅</t>
+    <t>唐毅</t>
   </si>
   <si>
     <t>赵江涛</t>
   </si>
   <si>
-    <t xml:space="preserve">　　姜宏</t>
+    <t>姜宏</t>
   </si>
   <si>
     <t>张佰成</t>
@@ -1006,13 +1006,13 @@
     <t>张晓兵</t>
   </si>
   <si>
-    <t xml:space="preserve">　　王旺盛</t>
+    <t>王旺盛</t>
   </si>
   <si>
     <t>郭玉峰</t>
   </si>
   <si>
-    <t xml:space="preserve">　　斯琴毕力格</t>
+    <t>斯琴毕力格</t>
   </si>
   <si>
     <t>王路</t>
@@ -1024,7 +1024,7 @@
     <t>于强</t>
   </si>
   <si>
-    <t xml:space="preserve">　　李明伟</t>
+    <t>李明伟</t>
   </si>
   <si>
     <t>孙弘</t>
@@ -1042,7 +1042,7 @@
     <t>郑莉</t>
   </si>
   <si>
-    <t xml:space="preserve">　　吴群刚</t>
+    <t>吴群刚</t>
   </si>
   <si>
     <t>杜紫平</t>
@@ -1066,7 +1066,7 @@
     <t>虞平</t>
   </si>
   <si>
-    <t xml:space="preserve">　　杨林兴</t>
+    <t>杨林兴</t>
   </si>
   <si>
     <t>胡元坤</t>
@@ -1087,7 +1087,7 @@
     <t>邓正权</t>
   </si>
   <si>
-    <t xml:space="preserve">　　邹瑾</t>
+    <t>邹瑾</t>
   </si>
   <si>
     <t>李晓波</t>
@@ -1099,13 +1099,13 @@
     <t>马汉成</t>
   </si>
   <si>
-    <t xml:space="preserve">　　张利</t>
-  </si>
-  <si>
-    <t xml:space="preserve">　　杨玉经</t>
-  </si>
-  <si>
-    <t xml:space="preserve">　　杜延安</t>
+    <t>张利</t>
+  </si>
+  <si>
+    <t>杨玉经</t>
+  </si>
+  <si>
+    <t>杜延安</t>
   </si>
   <si>
     <t>叶露中</t>
@@ -1114,22 +1114,22 @@
     <t>凌云</t>
   </si>
   <si>
-    <t xml:space="preserve">　　陈冰冰</t>
+    <t>陈冰冰</t>
   </si>
   <si>
     <t>孔晓宏</t>
   </si>
   <si>
-    <t xml:space="preserve">   操龙灿</t>
-  </si>
-  <si>
-    <t xml:space="preserve">　　戴启远</t>
+    <t>操龙灿</t>
+  </si>
+  <si>
+    <t>戴启远</t>
   </si>
   <si>
     <t>张孝成</t>
   </si>
   <si>
-    <t xml:space="preserve">　　许继伟</t>
+    <t>许继伟</t>
   </si>
   <si>
     <t>单向前</t>
@@ -1153,7 +1153,7 @@
     <t>孟庆斌</t>
   </si>
   <si>
-    <t xml:space="preserve">  张海波</t>
+    <t xml:space="preserve"> 张海波</t>
   </si>
   <si>
     <t>杨洪涛</t>
@@ -1180,7 +1180,7 @@
     <t>宇向东</t>
   </si>
   <si>
-    <t xml:space="preserve">　　田庆盈</t>
+    <t>田庆盈</t>
   </si>
   <si>
     <t>陈飞</t>
@@ -1195,7 +1195,7 @@
     <t>孟凡利</t>
   </si>
   <si>
-    <t xml:space="preserve">　　李云峰</t>
+    <t>李云峰</t>
   </si>
   <si>
     <t>王立伟</t>
@@ -1213,7 +1213,7 @@
     <t>王震</t>
   </si>
   <si>
-    <t xml:space="preserve">　　高键</t>
+    <t>高键</t>
   </si>
   <si>
     <t>储祥好</t>
@@ -1231,13 +1231,13 @@
     <t>危伟汉</t>
   </si>
   <si>
-    <t xml:space="preserve">　　朱伟</t>
-  </si>
-  <si>
-    <t xml:space="preserve">　　温国辉</t>
-  </si>
-  <si>
-    <t>刘吉　男</t>
+    <t>朱伟</t>
+  </si>
+  <si>
+    <t>温国辉</t>
+  </si>
+  <si>
+    <t>刘吉男</t>
   </si>
   <si>
     <t>张科</t>
@@ -1261,7 +1261,7 @@
     <t>陈如桂</t>
   </si>
   <si>
-    <t xml:space="preserve">　　马正勇</t>
+    <t>马正勇</t>
   </si>
   <si>
     <t>姜建军</t>
@@ -1273,7 +1273,7 @@
     <t>姚奕生</t>
   </si>
   <si>
-    <t xml:space="preserve">　　吕玉印</t>
+    <t>吕玉印</t>
   </si>
   <si>
     <t>袁古洁</t>
@@ -1294,7 +1294,7 @@
     <t>雷应敏</t>
   </si>
   <si>
-    <t xml:space="preserve">　　吴炜</t>
+    <t>吴炜</t>
   </si>
   <si>
     <t>秦春成</t>
@@ -1318,70 +1318,70 @@
     <t>林冠</t>
   </si>
   <si>
-    <t xml:space="preserve">　　谭丕创</t>
+    <t>谭丕创</t>
   </si>
   <si>
     <t>班忠柏</t>
   </si>
   <si>
-    <t xml:space="preserve">　　牙生·司地克</t>
-  </si>
-  <si>
-    <t xml:space="preserve">　　买买提明·卡德</t>
+    <t>牙生·司地克</t>
+  </si>
+  <si>
+    <t>买买提明·卡德</t>
   </si>
   <si>
     <t>韩立明</t>
   </si>
   <si>
-    <t xml:space="preserve">　　王晖</t>
+    <t>王晖</t>
   </si>
   <si>
     <t>王昊</t>
   </si>
   <si>
-    <t xml:space="preserve">　　陈金虎</t>
-  </si>
-  <si>
-    <t xml:space="preserve">　　庄兆林</t>
-  </si>
-  <si>
-    <t xml:space="preserve">　　张宝娟</t>
-  </si>
-  <si>
-    <t xml:space="preserve">　　杜小刚</t>
-  </si>
-  <si>
-    <t xml:space="preserve">　　朱立凡 现任泰州市委副书记</t>
-  </si>
-  <si>
-    <t xml:space="preserve">　　陈之常　男</t>
-  </si>
-  <si>
-    <t xml:space="preserve">　　曹路宝</t>
+    <t>陈金虎</t>
+  </si>
+  <si>
+    <t>庄兆林</t>
+  </si>
+  <si>
+    <t>张宝娟</t>
+  </si>
+  <si>
+    <t>杜小刚</t>
+  </si>
+  <si>
+    <t>朱立凡现任泰州市委副书记</t>
+  </si>
+  <si>
+    <t>陈之常男</t>
+  </si>
+  <si>
+    <t>曹路宝</t>
   </si>
   <si>
     <t>李亚平</t>
   </si>
   <si>
-    <t xml:space="preserve">　　方伟</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    朱晓明</t>
-  </si>
-  <si>
-    <t xml:space="preserve">陈云 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">　　谢来发</t>
-  </si>
-  <si>
-    <t xml:space="preserve">　　黄喜忠</t>
+    <t>方伟</t>
+  </si>
+  <si>
+    <t>朱晓明</t>
+  </si>
+  <si>
+    <t>陈云</t>
+  </si>
+  <si>
+    <t>谢来发</t>
+  </si>
+  <si>
+    <t>黄喜忠</t>
   </si>
   <si>
     <t>王少玄</t>
   </si>
   <si>
-    <t xml:space="preserve">　　许南吉</t>
+    <t>许南吉</t>
   </si>
   <si>
     <t>张鸿星</t>
@@ -1420,7 +1420,7 @@
     <t>梅世彤</t>
   </si>
   <si>
-    <t xml:space="preserve">　　邓沛然</t>
+    <t>邓沛然</t>
   </si>
   <si>
     <t>张瑞书</t>
@@ -1432,7 +1432,7 @@
     <t>董晓宇</t>
   </si>
   <si>
-    <t xml:space="preserve">　　张维亮</t>
+    <t>张维亮</t>
   </si>
   <si>
     <t>安伟</t>
@@ -1450,7 +1450,7 @@
     <t>张建慧</t>
   </si>
   <si>
-    <t xml:space="preserve">　　袁家健</t>
+    <t>袁家健</t>
   </si>
   <si>
     <t>张雷明</t>
@@ -1459,19 +1459,19 @@
     <t>高建军</t>
   </si>
   <si>
-    <t xml:space="preserve">　　王登喜</t>
-  </si>
-  <si>
-    <t xml:space="preserve">　　 刘宛康</t>
-  </si>
-  <si>
-    <t xml:space="preserve">　　刘尚进</t>
+    <t>王登喜</t>
+  </si>
+  <si>
+    <t>刘宛康</t>
+  </si>
+  <si>
+    <t>刘尚进</t>
   </si>
   <si>
     <t>杨青玖</t>
   </si>
   <si>
-    <t xml:space="preserve">　　徐衣显</t>
+    <t>徐衣显</t>
   </si>
   <si>
     <t>史根治</t>
@@ -1480,7 +1480,7 @@
     <t>王新伟</t>
   </si>
   <si>
-    <t xml:space="preserve">　　朱是西</t>
+    <t>朱是西</t>
   </si>
   <si>
     <t>郭浩</t>
@@ -1492,28 +1492,28 @@
     <t>吴海平</t>
   </si>
   <si>
-    <t xml:space="preserve">　　毛宏芳</t>
+    <t>毛宏芳</t>
   </si>
   <si>
     <t>裘东耀</t>
   </si>
   <si>
-    <t xml:space="preserve">　　刘忻</t>
+    <t>刘忻</t>
   </si>
   <si>
     <t>姚高员</t>
   </si>
   <si>
-    <t xml:space="preserve">　　王纲</t>
-  </si>
-  <si>
-    <t xml:space="preserve">　　盛阅春</t>
+    <t>王纲</t>
+  </si>
+  <si>
+    <t>盛阅春</t>
   </si>
   <si>
     <t>何中伟</t>
   </si>
   <si>
-    <t xml:space="preserve">　　汤飞帆</t>
+    <t>汤飞帆</t>
   </si>
   <si>
     <t>尹学群</t>
@@ -1570,7 +1570,7 @@
     <t>李爱武</t>
   </si>
   <si>
-    <t xml:space="preserve">　　曹立军</t>
+    <t>曹立军</t>
   </si>
   <si>
     <t>刘革安</t>
@@ -1579,7 +1579,7 @@
     <t>雷绍业</t>
   </si>
   <si>
-    <t xml:space="preserve">　　阳卫国</t>
+    <t>阳卫国</t>
   </si>
   <si>
     <t>朱洪武</t>
@@ -1594,22 +1594,22 @@
     <t>朱健</t>
   </si>
   <si>
-    <t xml:space="preserve">　　刘事青</t>
+    <t>刘事青</t>
   </si>
   <si>
     <t>刘志仁</t>
   </si>
   <si>
-    <t xml:space="preserve">　　郑建新</t>
+    <t>郑建新</t>
   </si>
   <si>
     <t>张伟文</t>
   </si>
   <si>
-    <t xml:space="preserve">　　王 军</t>
-  </si>
-  <si>
-    <t xml:space="preserve">　　戴超</t>
+    <t>王军</t>
+  </si>
+  <si>
+    <t>戴超</t>
   </si>
   <si>
     <t>王奋彦</t>
@@ -1639,7 +1639,7 @@
     <t>庄稼汉</t>
   </si>
   <si>
-    <t xml:space="preserve">　　梁伟新</t>
+    <t>梁伟新</t>
   </si>
   <si>
     <t>王永礼</t>
@@ -1654,7 +1654,7 @@
     <t>李建辉</t>
   </si>
   <si>
-    <t xml:space="preserve">　　林兴禄</t>
+    <t>林兴禄</t>
   </si>
   <si>
     <t>果果</t>
@@ -1663,7 +1663,7 @@
     <t>李刚</t>
   </si>
   <si>
-    <t xml:space="preserve">　　宋晓路</t>
+    <t>宋晓路</t>
   </si>
   <si>
     <t>张集智</t>
@@ -1672,7 +1672,7 @@
     <t>陈晏</t>
   </si>
   <si>
-    <t xml:space="preserve">　　黄伟</t>
+    <t>黄伟</t>
   </si>
   <si>
     <t>陈少荣</t>
@@ -1693,10 +1693,10 @@
     <t>姜有为</t>
   </si>
   <si>
-    <t xml:space="preserve">　　汤方栋</t>
-  </si>
-  <si>
-    <t xml:space="preserve">　　许桂清</t>
+    <t>汤方栋</t>
+  </si>
+  <si>
+    <t>许桂清</t>
   </si>
   <si>
     <t>王力威</t>
@@ -1705,10 +1705,10 @@
     <t>王一兵</t>
   </si>
   <si>
-    <t xml:space="preserve">　　隋显利</t>
-  </si>
-  <si>
-    <t xml:space="preserve">　　于学利</t>
+    <t>隋显利</t>
+  </si>
+  <si>
+    <t>于学利</t>
   </si>
   <si>
     <t>张成中</t>
@@ -1717,7 +1717,7 @@
     <t>卫华</t>
   </si>
   <si>
-    <t xml:space="preserve">　　郑光照</t>
+    <t>郑光照</t>
   </si>
   <si>
     <t>赵俊民</t>
@@ -1762,13 +1762,13 @@
     <t>孙喆</t>
   </si>
   <si>
-    <t xml:space="preserve">　　何忠华</t>
+    <t>何忠华</t>
   </si>
   <si>
     <t>王文力</t>
   </si>
   <si>
-    <t xml:space="preserve">　　 张子林</t>
+    <t>张子林</t>
   </si>
   <si>
     <t>于洪涛</t>
@@ -1777,7 +1777,7 @@
     <t>王秋实</t>
   </si>
   <si>
-    <t xml:space="preserve">　　李世峰</t>
+    <t>李世峰</t>
   </si>
   <si>
     <t>李玉刚</t>
@@ -8348,6 +8348,9 @@
       <c r="F121" t="s">
         <v>589</v>
       </c>
+      <c r="G121" t="s">
+        <v>592</v>
+      </c>
       <c r="H121" s="2">
         <v>24412</v>
       </c>
@@ -8875,6 +8878,9 @@
       <c r="E134" t="s">
         <v>446</v>
       </c>
+      <c r="F134" t="s">
+        <v>589</v>
+      </c>
       <c r="G134" t="s">
         <v>592</v>
       </c>
@@ -9039,6 +9045,9 @@
       <c r="F138" t="s">
         <v>590</v>
       </c>
+      <c r="G138" t="s">
+        <v>592</v>
+      </c>
       <c r="H138" s="2">
         <v>22190</v>
       </c>
@@ -9074,6 +9083,12 @@
       <c r="E139" t="s">
         <v>451</v>
       </c>
+      <c r="F139" t="s">
+        <v>589</v>
+      </c>
+      <c r="G139" t="s">
+        <v>592</v>
+      </c>
       <c r="H139" s="2">
         <v>28095</v>
       </c>
@@ -9106,6 +9121,9 @@
       <c r="F140" t="s">
         <v>589</v>
       </c>
+      <c r="G140" t="s">
+        <v>592</v>
+      </c>
       <c r="H140" s="2">
         <v>24807</v>
       </c>
@@ -10116,6 +10134,9 @@
       <c r="E165" t="s">
         <v>477</v>
       </c>
+      <c r="F165" t="s">
+        <v>589</v>
+      </c>
       <c r="G165" t="s">
         <v>592</v>
       </c>
@@ -12145,6 +12166,9 @@
       <c r="F215" t="s">
         <v>589</v>
       </c>
+      <c r="G215" t="s">
+        <v>592</v>
+      </c>
       <c r="H215" s="2">
         <v>23621</v>
       </c>
@@ -12593,6 +12617,9 @@
       <c r="F226" t="s">
         <v>589</v>
       </c>
+      <c r="G226" t="s">
+        <v>592</v>
+      </c>
       <c r="H226" s="2">
         <v>25842</v>
       </c>
@@ -12754,6 +12781,9 @@
       <c r="F230" t="s">
         <v>589</v>
       </c>
+      <c r="G230" t="s">
+        <v>592</v>
+      </c>
       <c r="H230" s="2">
         <v>31959</v>
       </c>
@@ -12871,6 +12901,9 @@
       <c r="F233" t="s">
         <v>589</v>
       </c>
+      <c r="G233" t="s">
+        <v>592</v>
+      </c>
       <c r="H233" s="2">
         <v>23316</v>
       </c>
@@ -13193,6 +13226,9 @@
       <c r="F241" t="s">
         <v>589</v>
       </c>
+      <c r="G241" t="s">
+        <v>592</v>
+      </c>
       <c r="H241" s="2">
         <v>24412</v>
       </c>
@@ -13272,6 +13308,9 @@
       <c r="F243" t="s">
         <v>589</v>
       </c>
+      <c r="G243" t="s">
+        <v>592</v>
+      </c>
       <c r="H243" s="2">
         <v>25965</v>
       </c>
@@ -13593,6 +13632,12 @@
       </c>
       <c r="E251" t="s">
         <v>563</v>
+      </c>
+      <c r="F251" t="s">
+        <v>589</v>
+      </c>
+      <c r="G251" t="s">
+        <v>592</v>
       </c>
       <c r="H251" s="2">
         <v>23408</v>

</xml_diff>